<commit_message>
rename, update, done eda/ml
</commit_message>
<xml_diff>
--- a/data/flight_dataset_description.xlsx
+++ b/data/flight_dataset_description.xlsx
@@ -865,7 +865,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -875,6 +875,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -943,7 +949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -976,6 +982,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1312,10 +1321,10 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,7 +1345,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1347,7 +1356,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1356,7 +1365,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1365,7 +1374,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1374,7 +1383,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1383,7 +1392,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1392,7 +1401,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1401,7 +1410,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1410,7 +1419,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1419,7 +1428,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1428,7 +1437,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>66</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1439,7 +1448,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1448,7 +1457,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1457,7 +1466,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -1466,7 +1475,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1475,7 +1484,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>67</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1486,7 +1495,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1495,7 +1504,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
@@ -1504,7 +1513,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1513,7 +1522,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
@@ -1522,7 +1531,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>68</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1533,7 +1542,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
@@ -1542,7 +1551,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="3" t="s">
         <v>24</v>
       </c>
@@ -1551,7 +1560,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>69</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1562,7 +1571,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
@@ -1571,7 +1580,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
@@ -1580,7 +1589,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="3" t="s">
         <v>28</v>
       </c>
@@ -1589,7 +1598,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="13" t="s">
         <v>71</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1600,7 +1609,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
@@ -1609,7 +1618,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="3" t="s">
         <v>31</v>
       </c>
@@ -1618,7 +1627,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="3" t="s">
         <v>32</v>
       </c>
@@ -1627,7 +1636,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="3" t="s">
         <v>33</v>
       </c>
@@ -1653,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1666,10 +1675,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>73</v>
       </c>
       <c r="C1" s="11" t="s">
@@ -1677,36 +1686,36 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="11" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="11" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="11" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="11" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="19" t="s">
         <v>74</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -1714,36 +1723,36 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="19" t="s">
         <v>80</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1751,29 +1760,29 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="11" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="19" t="s">
         <v>85</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -1781,31 +1790,31 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="11" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="11" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="19" t="s">
         <v>91</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -1813,64 +1822,64 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="11" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="19"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="11" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="19"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="18" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -1878,173 +1887,173 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="11" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="19"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="11" t="s">
+      <c r="A31" s="18"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="12" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="6" t="s">
+      <c r="A33" s="17"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="11" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="6" t="s">
+      <c r="A34" s="17"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="16"/>
-      <c r="B35" s="18" t="s">
+      <c r="A35" s="17"/>
+      <c r="B35" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="6" t="s">
+      <c r="A36" s="17"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="6" t="s">
+      <c r="A37" s="17"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="18" t="s">
+      <c r="A38" s="17"/>
+      <c r="B38" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="11" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="6" t="s">
+      <c r="A39" s="18"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="11" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="11" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="16"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="6" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="11" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="6" t="s">
+      <c r="A42" s="17"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="11" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="16"/>
-      <c r="B43" s="18" t="s">
+      <c r="A43" s="17"/>
+      <c r="B43" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="11" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="6" t="s">
+      <c r="A44" s="17"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="16"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="6" t="s">
+      <c r="A45" s="17"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="6" t="s">
+      <c r="A46" s="17"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="11" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="16"/>
-      <c r="B47" s="18" t="s">
+      <c r="A47" s="17"/>
+      <c r="B47" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="11" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="16"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="6" t="s">
+      <c r="A48" s="17"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="11" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
-      <c r="B49" s="18" t="s">
+      <c r="A49" s="17"/>
+      <c r="B49" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="11" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="17"/>
-      <c r="B50" s="20"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="21"/>
       <c r="C50" s="6" t="s">
         <v>132</v>
       </c>

</xml_diff>